<commit_message>
first full draft of new metrics
</commit_message>
<xml_diff>
--- a/Metrics TraceTree.xlsx
+++ b/Metrics TraceTree.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgrimes/Desktop/VPCShare/TMT/newstufflocal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgrimes/Desktop/VPCShare/TMT/TraceTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119DFE87-71AB-EB41-841C-C2C85CC16BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E5529C-88B4-1646-8157-C6E8062A46A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10580" yWindow="11000" windowWidth="20780" windowHeight="10000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pages" sheetId="2" r:id="rId1"/>
     <sheet name="Metrics" sheetId="1" r:id="rId2"/>
+    <sheet name="side-by-side" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metrics!$B$2:$F$21</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="109">
   <si>
     <t>Module</t>
   </si>
@@ -426,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,8 +474,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +512,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -514,15 +528,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,8 +581,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -864,28 +884,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="4" spans="1:2" ht="16" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
@@ -928,18 +948,18 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="15"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -955,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1752,4 +1772,427 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79192D7-8615-6B45-8665-5BC457AC5437}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="K4" sqref="A4:K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" customWidth="1"/>
+    <col min="15" max="15" width="35.83203125" customWidth="1"/>
+    <col min="16" max="16" width="2.83203125" style="16" customWidth="1"/>
+    <col min="17" max="17" width="6.1640625" customWidth="1"/>
+    <col min="18" max="18" width="22.83203125" customWidth="1"/>
+    <col min="19" max="19" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="51">
+      <c r="A1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="17">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="17">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="34">
+      <c r="A4" s="1"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="14"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="14"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="14"/>
+      <c r="M4" s="1">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" ht="34">
+      <c r="A5" s="1">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1">
+        <v>13</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1">
+        <v>13</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="1">
+        <v>13</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="34">
+      <c r="A6" s="1">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="14"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="14"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" ht="17">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="34">
+      <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="1">
+        <v>19</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="1">
+        <v>19</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17">
+      <c r="A9" s="1">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="14"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" ht="17">
+      <c r="A10" s="1">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1">
+        <v>18</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="1">
+        <v>18</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="1"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="1"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="1"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>